<commit_message>
our updated scrum document
</commit_message>
<xml_diff>
--- a/tools and methods.xlsx
+++ b/tools and methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c8053f95979199d/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="668" documentId="13_ncr:1_{D4C88E90-DDAE-41BA-BC90-4BFFBC8F73D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4A4C0EE0-9535-41EE-A2AD-8D0C75703608}"/>
+  <xr:revisionPtr revIDLastSave="702" documentId="13_ncr:1_{D4C88E90-DDAE-41BA-BC90-4BFFBC8F73D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B0DC7A25-5540-470F-8E58-9A0447D62AF2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="95">
   <si>
     <t>STATUS</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Participants</t>
   </si>
   <si>
-    <t xml:space="preserve">Location </t>
-  </si>
-  <si>
     <t>Online</t>
   </si>
   <si>
@@ -129,15 +126,9 @@
     <t xml:space="preserve">As a user , I can take a part in the survey. </t>
   </si>
   <si>
-    <t xml:space="preserve">As a user,  I can select best option fro the question. </t>
-  </si>
-  <si>
     <t>As a user, I can see the my survey result.</t>
   </si>
   <si>
-    <t>As a user, I can see my result comparing with candidates choice.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Task : Make a question on rough paper </t>
   </si>
   <si>
@@ -168,12 +159,6 @@
     <t xml:space="preserve">Bawan </t>
   </si>
   <si>
-    <t>As a user, I should be able to start the main page and continue the survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a Participants, I can able to start the main page </t>
-  </si>
-  <si>
     <t xml:space="preserve">As a Participants ,I am able to  delete the question and the option. </t>
   </si>
   <si>
@@ -186,12 +171,6 @@
     <t>As a Participants , I can add, edit  the question.</t>
   </si>
   <si>
-    <t>As a Participants, I am able to check the users question</t>
-  </si>
-  <si>
-    <t>As a Participants , I am able to tally the question and user's answers.</t>
-  </si>
-  <si>
     <t>As a user, I am able to choose freely given options from the survey.</t>
   </si>
   <si>
@@ -204,18 +183,12 @@
     <t>Shantosh</t>
   </si>
   <si>
-    <t>Siva</t>
-  </si>
-  <si>
     <t>Bawan</t>
   </si>
   <si>
     <t xml:space="preserve">Task : made sample of project </t>
   </si>
   <si>
-    <t xml:space="preserve">Task: devided task as intrest </t>
-  </si>
-  <si>
     <t xml:space="preserve">Task: Plan how to start the project </t>
   </si>
   <si>
@@ -225,27 +198,15 @@
     <t>Task: made formate for the output of survey.</t>
   </si>
   <si>
-    <t>Task: made sql tabl formate.</t>
-  </si>
-  <si>
     <t>Task : insert the required data to mysql database.</t>
   </si>
   <si>
     <t>Task: made required questions for the survey.</t>
   </si>
   <si>
-    <t xml:space="preserve">Task : made dao file for main part </t>
-  </si>
-  <si>
     <t xml:space="preserve">Task : select some related images for the project </t>
   </si>
   <si>
-    <t xml:space="preserve">Task : Place those images in right place </t>
-  </si>
-  <si>
-    <t>Task : collect diffrent data from different sources.</t>
-  </si>
-  <si>
     <t>Week 15</t>
   </si>
   <si>
@@ -261,18 +222,9 @@
     <t>Task: made Qdao file for questions</t>
   </si>
   <si>
-    <t>Task : Make a Qdelete file for delete questions.</t>
-  </si>
-  <si>
-    <t>Task : make a showquestions java file for show questions.</t>
-  </si>
-  <si>
     <t>Task : Newquestion jsp file for questiosns</t>
   </si>
   <si>
-    <t xml:space="preserve">Task: made question.java file </t>
-  </si>
-  <si>
     <t xml:space="preserve">Task: made showquestions.java file </t>
   </si>
   <si>
@@ -306,22 +258,67 @@
     <t xml:space="preserve">Task : make read to update file </t>
   </si>
   <si>
-    <t xml:space="preserve">Task : made somehtml file </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task: make index file for jsp  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task: link all made file to main project </t>
-  </si>
-  <si>
     <t xml:space="preserve">shantosh </t>
   </si>
   <si>
-    <t xml:space="preserve">Task: made new question.jsp file for questions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task : make show participants .jsp file </t>
+    <t>As a user, I should be able to start the main page and continue the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user,  I can select best option for the questions. </t>
+  </si>
+  <si>
+    <t>As a user, I can see my result comparing with participants choice.</t>
+  </si>
+  <si>
+    <t>As a Participants, I can able to start the main page.</t>
+  </si>
+  <si>
+    <t>As a Participants, I am able to check the users questions.</t>
+  </si>
+  <si>
+    <t>As a Participants , I am able to tally the questions and user's answers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: divided task as interest </t>
+  </si>
+  <si>
+    <t>Task: made sql tabl format.</t>
+  </si>
+  <si>
+    <t>Shiva</t>
+  </si>
+  <si>
+    <t>Task : collect data from different sources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task : Place selected images in right place </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task : made dao connection file for main part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: made showquestion.jsp file </t>
+  </si>
+  <si>
+    <t>Task : Made a Qdelete file for delete questions.</t>
+  </si>
+  <si>
+    <t>Task : Made a showquestions jsp file for show questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: Made index.jsp file and insertdata java file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task : make showparticipants .jsp file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task : made somehtml and style.css file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task: Made showparticipants.java file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task:  made newquestion.jsp file for questions </t>
   </si>
 </sst>
 </file>
@@ -623,6 +620,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,9 +630,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1369,7 +1366,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1402,7 +1399,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1800" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1432,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1469,7 +1466,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1784,7 +1781,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="1" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1817,7 +1814,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1851,7 +1848,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1886,7 +1883,7 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2244,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41624483-528A-487E-8318-BAE844736E7C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2259,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95158496-5B07-4778-871C-839C6BA690D9}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2272,19 +2269,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -2292,7 +2289,7 @@
     </row>
     <row r="3" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -2301,18 +2298,18 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -2332,7 +2329,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -2343,7 +2340,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -2354,13 +2351,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2373,7 +2370,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
@@ -2384,7 +2381,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -2395,7 +2392,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2">
         <v>3</v>
@@ -2406,7 +2403,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
@@ -2417,7 +2414,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
@@ -2432,7 +2429,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
@@ -2443,7 +2440,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2">
         <v>3</v>
@@ -2454,7 +2451,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
@@ -2465,7 +2462,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -2476,7 +2473,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
@@ -2645,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6088DA-74CF-4F3C-ACDE-C67EABB84574}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2658,55 +2655,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>17</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -2744,16 +2741,16 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="14">
         <v>2</v>
@@ -2762,7 +2759,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="14">
         <v>1</v>
@@ -2783,16 +2780,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="14">
         <v>2</v>
@@ -2822,16 +2819,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="14">
         <v>2</v>
@@ -2842,7 +2839,9 @@
       <c r="G6" s="14">
         <v>1</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="14">
+        <v>2</v>
+      </c>
       <c r="I6" s="14">
         <v>2</v>
       </c>
@@ -2859,16 +2858,16 @@
     </row>
     <row r="7" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14">
         <v>2</v>
@@ -2898,7 +2897,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -2920,17 +2919,17 @@
       <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
-        <v>58</v>
+      <c r="A9" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="14">
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="14">
         <v>2</v>
@@ -2959,17 +2958,17 @@
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>59</v>
+      <c r="A10" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="14">
         <v>2</v>
@@ -2998,17 +2997,17 @@
       <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>60</v>
+      <c r="A11" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="B11" s="14">
         <v>4</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="14">
         <v>2</v>
@@ -3037,17 +3036,17 @@
       <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>61</v>
+      <c r="A12" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="14">
         <v>1</v>
@@ -3077,7 +3076,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -3100,16 +3099,16 @@
     </row>
     <row r="14" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B14" s="14">
         <v>2</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="14">
         <v>2</v>
@@ -3139,16 +3138,16 @@
     </row>
     <row r="15" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" s="14">
         <v>3</v>
@@ -3178,16 +3177,16 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B16" s="14">
         <v>2</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" s="14">
         <v>2</v>
@@ -3217,16 +3216,16 @@
     </row>
     <row r="17" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" s="14">
         <v>2</v>
@@ -3256,7 +3255,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -3277,18 +3276,18 @@
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B19" s="14">
         <v>4</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E19" s="14">
         <v>2</v>
@@ -3318,16 +3317,16 @@
     </row>
     <row r="20" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20" s="14">
         <v>1</v>
@@ -3355,18 +3354,18 @@
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
     </row>
-    <row r="21" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B21" s="14">
         <v>4</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" s="14">
         <v>2</v>
@@ -3396,16 +3395,16 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B22" s="14">
         <v>4</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E22" s="14">
         <v>1</v>
@@ -3435,7 +3434,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
@@ -3458,16 +3457,16 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" s="14">
         <v>2</v>
@@ -3497,16 +3496,16 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B25" s="14">
         <v>4</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E25" s="14">
         <v>4</v>
@@ -3536,16 +3535,16 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B26" s="14">
         <v>4</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E26" s="14">
         <v>2</v>
@@ -3575,16 +3574,16 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" s="14">
         <v>2</v>
@@ -3614,7 +3613,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -3629,11 +3628,11 @@
       </c>
       <c r="G28" s="10">
         <f>SUM(G3:G27)</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="10">
         <f>SUM(H3:H27)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I28" s="10">
         <f>SUM(I3:I27)</f>
@@ -3664,7 +3663,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3686,39 +3685,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E2" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3740,19 +3739,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3760,16 +3759,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -3791,19 +3790,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3811,16 +3810,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3842,19 +3841,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3862,16 +3861,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3893,19 +3892,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3913,16 +3912,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -3949,7 +3948,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3961,55 +3960,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="A1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>17</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -4024,7 +4023,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -4047,16 +4046,16 @@
     </row>
     <row r="4" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="14">
         <v>2</v>
@@ -4086,16 +4085,16 @@
     </row>
     <row r="5" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="14">
         <v>2</v>
@@ -4125,16 +4124,16 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="14">
         <v>2</v>
@@ -4162,18 +4161,18 @@
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14">
         <v>2</v>
@@ -4203,7 +4202,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
@@ -4226,16 +4225,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B9" s="14">
         <v>2</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="14">
         <v>3</v>
@@ -4265,16 +4264,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B10" s="14">
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="14">
         <v>2</v>
@@ -4304,16 +4303,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="14">
         <v>2</v>
@@ -4343,16 +4342,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B12" s="14">
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="14">
         <v>2</v>
@@ -4382,7 +4381,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -4405,16 +4404,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B14" s="14">
         <v>4</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="14">
         <v>3</v>
@@ -4444,16 +4443,16 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B15" s="14">
         <v>4</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" s="14">
         <v>2</v>
@@ -4489,10 +4488,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E16" s="14">
         <v>2</v>
@@ -4522,16 +4521,16 @@
     </row>
     <row r="17" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B17" s="14">
         <v>4</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" s="14">
         <v>2</v>
@@ -4561,7 +4560,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -4584,16 +4583,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B19" s="14">
         <v>4</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E19" s="14">
         <v>2</v>
@@ -4623,16 +4622,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B20" s="14">
         <v>4</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20" s="14">
         <v>2</v>
@@ -4662,16 +4661,16 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B21" s="14">
         <v>4</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>55</v>
+      <c r="C21" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" s="14">
         <v>4</v>
@@ -4701,16 +4700,16 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B22" s="14">
         <v>4</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E22" s="14">
         <v>4</v>
@@ -4740,7 +4739,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
@@ -4763,16 +4762,16 @@
     </row>
     <row r="24" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B24" s="14">
         <v>2</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" s="14">
         <v>3</v>
@@ -4802,16 +4801,16 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B25" s="14">
         <v>2</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E25" s="14">
         <v>3</v>
@@ -4841,16 +4840,16 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B26" s="14">
         <v>2</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E26" s="14">
         <v>4</v>
@@ -4880,16 +4879,16 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" s="14">
         <v>4</v>
@@ -4897,7 +4896,9 @@
       <c r="F27" s="14">
         <v>4</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="14">
+        <v>4</v>
+      </c>
       <c r="H27" s="14">
         <v>4</v>
       </c>
@@ -4917,7 +4918,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -4932,7 +4933,7 @@
       </c>
       <c r="G28" s="10">
         <f>SUM(G3:G27)</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H28" s="10">
         <f>SUM(H3:H27)</f>

</xml_diff>